<commit_message>
Actualizacion de inmuebles 16-01-2025
</commit_message>
<xml_diff>
--- a/public/usuarios.xlsx
+++ b/public/usuarios.xlsx
@@ -15,24 +15,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>202cb962ac59075b964b07152d234b70</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Inmueble</t>
+  </si>
+  <si>
+    <t>fecha_apertura</t>
+  </si>
+  <si>
+    <t>fecha_cierre</t>
+  </si>
+  <si>
+    <t>comentario</t>
+  </si>
+  <si>
+    <t>PRUEBA</t>
+  </si>
+  <si>
+    <t>2025-01-14</t>
+  </si>
+  <si>
+    <t>0000-00-00</t>
+  </si>
+  <si>
+    <t>WWW</t>
+  </si>
+  <si>
+    <t>2025-01-15</t>
+  </si>
+  <si>
+    <t>asww</t>
+  </si>
+  <si>
+    <t>2025-01-31</t>
+  </si>
+  <si>
+    <t>qqqqqqqqqqq</t>
   </si>
 </sst>
 </file>
@@ -372,7 +390,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,14 +413,45 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>